<commit_message>
Modified UX and changed gpa calculation to 2 dimensional list approach
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2469f11167be8cd/Desktop/5001_Python/CollegeAdministration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{39E4DEDB-2077-4343-B5C7-B2D7337F35DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{39E4DEDB-2077-4343-B5C7-B2D7337F35DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{316E5732-3171-4B95-8507-E930578387B7}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2376560A-06F7-40BA-B55D-52ADD451EC61}"/>
   </bookViews>
@@ -127,6 +127,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -429,10 +433,13 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -485,22 +492,22 @@
         <v>8</v>
       </c>
       <c r="B3" s="2">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2">
+        <v>87</v>
+      </c>
+      <c r="D3" s="2">
+        <v>89</v>
+      </c>
+      <c r="E3" s="2">
+        <v>90</v>
+      </c>
+      <c r="F3" s="2">
         <v>88</v>
       </c>
-      <c r="D3" s="2">
-        <v>91</v>
-      </c>
-      <c r="E3" s="2">
-        <v>79</v>
-      </c>
-      <c r="F3" s="2">
-        <v>85</v>
-      </c>
       <c r="G3" s="2">
-        <v>90</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added report generation and download
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d2469f11167be8cd/Desktop/5001_Python/CollegeAdministration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{39E4DEDB-2077-4343-B5C7-B2D7337F35DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{316E5732-3171-4B95-8507-E930578387B7}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{39E4DEDB-2077-4343-B5C7-B2D7337F35DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02678F8D-EECA-401A-AD59-9611E4E27D3E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{2376560A-06F7-40BA-B55D-52ADD451EC61}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Student Name</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>Vikram</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Alice</t>
   </si>
 </sst>
 </file>
@@ -430,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13D8B909-A586-44B6-844A-D270E2A2B8DE}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="A6" sqref="A6:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,22 +475,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="2">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C2" s="2">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E2" s="2">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="F2" s="2">
-        <v>92</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -509,6 +515,286 @@
       <c r="G3" s="2">
         <v>98</v>
       </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2">
+        <v>69</v>
+      </c>
+      <c r="C4" s="2">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>